<commit_message>
finished rerunning through code!
</commit_message>
<xml_diff>
--- a/Data_Files/SupDataset3_BP_GOterms_of_interest.xlsx
+++ b/Data_Files/SupDataset3_BP_GOterms_of_interest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariaingersoll/Desktop/BU_Research/Davies-Gilmore/Aip_FS_2022/Aiptasia_Fed_Starved/Data_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C79BD54-151F-C941-BFED-B9AE5200A615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2390C339-5EA3-6E41-A5D7-69FFDD482B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="980" windowWidth="22800" windowHeight="15880" activeTab="1" xr2:uid="{BD502E35-1F59-A342-8A51-7D9BBB58FBF6}"/>
+    <workbookView xWindow="5620" yWindow="960" windowWidth="22800" windowHeight="15880" activeTab="1" xr2:uid="{BD502E35-1F59-A342-8A51-7D9BBB58FBF6}"/>
   </bookViews>
   <sheets>
     <sheet name="BPapo_aip" sheetId="4" r:id="rId1"/>
@@ -5557,7 +5557,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>